<commit_message>
Recalibrate BTCC and EoTCCwTC
</commit_message>
<xml_diff>
--- a/InputData/elec/EoTCCwTC/Elasticity of TCC wrt Transmission Capacity.xlsx
+++ b/InputData/elec/EoTCCwTC/Elasticity of TCC wrt Transmission Capacity.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\elec\EoTCCwTC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\elec\EoTCCwTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>a physical build-out of the system) and change in the Transmission</t>
   </si>
@@ -158,18 +158,9 @@
     <t>Onshore wind GW</t>
   </si>
   <si>
-    <t>Offshore wind GW</t>
-  </si>
-  <si>
     <t>Onshore wind Curtailment</t>
   </si>
   <si>
-    <t>2021 BTCC Value</t>
-  </si>
-  <si>
-    <t>Offshore wind</t>
-  </si>
-  <si>
     <t>Greening the Grid</t>
   </si>
   <si>
@@ -177,6 +168,27 @@
   </si>
   <si>
     <t>Figure 63</t>
+  </si>
+  <si>
+    <t>2025 BTCC Value</t>
+  </si>
+  <si>
+    <t>Time (Year)</t>
+  </si>
+  <si>
+    <t>Output Electricity Generation Capacity[onshore wind es] : NoSettings</t>
+  </si>
+  <si>
+    <t>Output Electricity Generation Capacity[solar PV es] : NoSettings</t>
+  </si>
+  <si>
+    <t>Perc Reduction in Cap Factor due to Flexibility Point Constraints[onshore wind es] : NoSettings</t>
+  </si>
+  <si>
+    <t>Perc Reduction in Cap Factor due to Flexibility Point Constraints[solar PV es] : NoSettings</t>
+  </si>
+  <si>
+    <t>We calibrated the EoTCCwTC variable for India based on the cited NREL study.</t>
   </si>
 </sst>
 </file>
@@ -184,7 +196,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -272,11 +284,11 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -287,8 +299,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -605,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -641,17 +654,17 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
@@ -732,6 +745,11 @@
     <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -745,10 +763,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO40"/>
+  <dimension ref="A1:AO53"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -772,7 +790,7 @@
         <v>27</v>
       </c>
       <c r="B4">
-        <v>2021</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -780,7 +798,7 @@
         <v>37</v>
       </c>
       <c r="B6">
-        <v>100.96</v>
+        <v>93.823999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -788,105 +806,177 @@
         <v>38</v>
       </c>
       <c r="B7">
-        <v>64.462999999999994</v>
+        <v>60.787999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B8">
-        <v>5.48</v>
+        <v>1.6329799999999998E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B9">
-        <v>1.7924900000000001E-2</v>
+        <v>9.9961300000000006E-3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10">
-        <v>1.00695E-2</v>
-      </c>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.42</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B12" s="3"/>
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3">
+        <f>B8*(B6/SUM(B6:B7))+B9*(B7/SUM(B6:B7))</f>
+        <v>1.3839623739683853E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0.35</v>
-      </c>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="3">
-        <f>(B6*B9+B7*B10+B8*B11)/SUM(B6:B8)</f>
-        <v>1.438715576964711E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B15" s="3"/>
+      <c r="A14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="10"/>
-    </row>
-    <row r="17" spans="1:41" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B16" s="3">
         <v>1.6E-2</v>
       </c>
     </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1.2E-2</v>
+      </c>
+    </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="3">
-        <v>1.2E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A21" s="10" t="s">
+      <c r="A19" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="10"/>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:41" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="12">
+        <v>0.42</v>
+      </c>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+      <c r="AB20"/>
+      <c r="AC20"/>
+      <c r="AD20"/>
+      <c r="AE20"/>
+      <c r="AF20"/>
+      <c r="AG20"/>
+      <c r="AH20"/>
+      <c r="AI20"/>
+      <c r="AJ20"/>
+      <c r="AK20"/>
+      <c r="AL20"/>
+      <c r="AM20"/>
+      <c r="AN20"/>
+      <c r="AO20"/>
+    </row>
+    <row r="21" spans="1:41" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+      <c r="AB21"/>
+      <c r="AC21"/>
+      <c r="AD21"/>
+      <c r="AE21"/>
+      <c r="AF21"/>
+      <c r="AG21"/>
+      <c r="AH21"/>
+      <c r="AI21"/>
+      <c r="AJ21"/>
+      <c r="AK21"/>
+      <c r="AL21"/>
+      <c r="AM21"/>
+      <c r="AN21"/>
+      <c r="AO21"/>
     </row>
     <row r="22" spans="1:41" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="13">
-        <v>0.5</v>
-      </c>
+      <c r="A22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22"/>
@@ -927,211 +1017,1321 @@
       <c r="AN22"/>
       <c r="AO22"/>
     </row>
-    <row r="23" spans="1:41" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23"/>
-      <c r="N23"/>
-      <c r="O23"/>
-      <c r="P23"/>
-      <c r="Q23"/>
-      <c r="R23"/>
-      <c r="S23"/>
-      <c r="T23"/>
-      <c r="U23"/>
-      <c r="V23"/>
-      <c r="W23"/>
-      <c r="X23"/>
-      <c r="Y23"/>
-      <c r="Z23"/>
-      <c r="AA23"/>
-      <c r="AB23"/>
-      <c r="AC23"/>
-      <c r="AD23"/>
-      <c r="AE23"/>
-      <c r="AF23"/>
-      <c r="AG23"/>
-      <c r="AH23"/>
-      <c r="AI23"/>
-      <c r="AJ23"/>
-      <c r="AK23"/>
-      <c r="AL23"/>
-      <c r="AM23"/>
-      <c r="AN23"/>
-      <c r="AO23"/>
-    </row>
-    <row r="24" spans="1:41" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-      <c r="N24"/>
-      <c r="O24"/>
-      <c r="P24"/>
-      <c r="Q24"/>
-      <c r="R24"/>
-      <c r="S24"/>
-      <c r="T24"/>
-      <c r="U24"/>
-      <c r="V24"/>
-      <c r="W24"/>
-      <c r="X24"/>
-      <c r="Y24"/>
-      <c r="Z24"/>
-      <c r="AA24"/>
-      <c r="AB24"/>
-      <c r="AC24"/>
-      <c r="AD24"/>
-      <c r="AE24"/>
-      <c r="AF24"/>
-      <c r="AG24"/>
-      <c r="AH24"/>
-      <c r="AI24"/>
-      <c r="AJ24"/>
-      <c r="AK24"/>
-      <c r="AL24"/>
-      <c r="AM24"/>
-      <c r="AN24"/>
-      <c r="AO24"/>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23">
+        <f>H40</f>
+        <v>93.218000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24">
+        <f>H39</f>
+        <v>61.063000000000002</v>
+      </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B25">
-        <v>64.757999999999996</v>
+        <f>H44</f>
+        <v>1.9394399999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26">
-        <v>103.036</v>
+        <f>H43</f>
+        <v>1.1796299999999999E-2</v>
       </c>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27">
-        <v>5.47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28">
-        <v>2.34719E-2</v>
+      <c r="A27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="14">
+        <f>B25*(B23/SUM(B23:B24))+B26*(B24/SUM(B23:B24))</f>
+        <v>1.6387141942948255E-2</v>
       </c>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29">
-        <v>1.2870299999999999E-2</v>
+      <c r="A29" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <f>H49</f>
+        <v>94.668000000000006</v>
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.45">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31">
+        <f>H48</f>
+        <v>60.497999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32">
+        <f>H53</f>
+        <v>1.40564E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33">
+        <f>H52</f>
+        <v>8.4487599999999996E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="12">
-        <f>(B25*B28+B26*B29+B27*B30)/SUM(B25:B27)</f>
-        <v>1.6426363993674392E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34">
-        <v>99.358000000000004</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35">
-        <v>64.227999999999994</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36">
-        <v>5.4749999999999996</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37">
-        <v>1.4445680000000001E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B34" s="14">
+        <f>B32*(B30/SUM(B30:B31))+B33*(B31/SUM(B30:B31))</f>
+        <v>1.1870025377208925E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A37" s="13">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B38">
-        <v>8.2466299999999996E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+        <v>2019</v>
+      </c>
+      <c r="C38">
+        <v>2020</v>
+      </c>
+      <c r="D38">
+        <v>2021</v>
+      </c>
+      <c r="E38">
+        <v>2022</v>
+      </c>
+      <c r="F38">
+        <v>2023</v>
+      </c>
+      <c r="G38">
+        <v>2024</v>
+      </c>
+      <c r="H38">
+        <v>2025</v>
+      </c>
+      <c r="I38">
+        <v>2026</v>
+      </c>
+      <c r="J38">
+        <v>2027</v>
+      </c>
+      <c r="K38">
+        <v>2028</v>
+      </c>
+      <c r="L38">
+        <v>2029</v>
+      </c>
+      <c r="M38">
+        <v>2030</v>
+      </c>
+      <c r="N38">
+        <v>2031</v>
+      </c>
+      <c r="O38">
+        <v>2032</v>
+      </c>
+      <c r="P38">
+        <v>2033</v>
+      </c>
+      <c r="Q38">
+        <v>2034</v>
+      </c>
+      <c r="R38">
+        <v>2035</v>
+      </c>
+      <c r="S38">
+        <v>2036</v>
+      </c>
+      <c r="T38">
+        <v>2037</v>
+      </c>
+      <c r="U38">
+        <v>2038</v>
+      </c>
+      <c r="V38">
+        <v>2039</v>
+      </c>
+      <c r="W38">
+        <v>2040</v>
+      </c>
+      <c r="X38">
+        <v>2041</v>
+      </c>
+      <c r="Y38">
+        <v>2042</v>
+      </c>
+      <c r="Z38">
+        <v>2043</v>
+      </c>
+      <c r="AA38">
+        <v>2044</v>
+      </c>
+      <c r="AB38">
+        <v>2045</v>
+      </c>
+      <c r="AC38">
+        <v>2046</v>
+      </c>
+      <c r="AD38">
+        <v>2047</v>
+      </c>
+      <c r="AE38">
+        <v>2048</v>
+      </c>
+      <c r="AF38">
+        <v>2049</v>
+      </c>
+      <c r="AG38">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B40" s="12">
-        <f>(B34*B37+B35*B38+B36*B39)/SUM(B34:B36)</f>
-        <v>1.1622777725672981E-2</v>
+        <v>35.213000000000001</v>
+      </c>
+      <c r="C39">
+        <v>37.707999999999998</v>
+      </c>
+      <c r="D39">
+        <v>40.203000000000003</v>
+      </c>
+      <c r="E39">
+        <v>44.097999999999999</v>
+      </c>
+      <c r="F39">
+        <v>49.192999999999998</v>
+      </c>
+      <c r="G39">
+        <v>55.082999999999998</v>
+      </c>
+      <c r="H39">
+        <v>61.063000000000002</v>
+      </c>
+      <c r="I39">
+        <v>67.647999999999996</v>
+      </c>
+      <c r="J39">
+        <v>74.858000000000004</v>
+      </c>
+      <c r="K39">
+        <v>81.933000000000007</v>
+      </c>
+      <c r="L39">
+        <v>88.367999999999995</v>
+      </c>
+      <c r="M39">
+        <v>95.492999999999995</v>
+      </c>
+      <c r="N39">
+        <v>105.328</v>
+      </c>
+      <c r="O39">
+        <v>117.108</v>
+      </c>
+      <c r="P39">
+        <v>131.148</v>
+      </c>
+      <c r="Q39">
+        <v>147.38300000000001</v>
+      </c>
+      <c r="R39">
+        <v>164.94300000000001</v>
+      </c>
+      <c r="S39">
+        <v>183.72300000000001</v>
+      </c>
+      <c r="T39">
+        <v>204.16300000000001</v>
+      </c>
+      <c r="U39">
+        <v>226.93799999999999</v>
+      </c>
+      <c r="V39">
+        <v>251.09299999999999</v>
+      </c>
+      <c r="W39">
+        <v>277.28300000000002</v>
+      </c>
+      <c r="X39">
+        <v>305.50299999999999</v>
+      </c>
+      <c r="Y39">
+        <v>335.928</v>
+      </c>
+      <c r="Z39">
+        <v>366.72800000000001</v>
+      </c>
+      <c r="AA39">
+        <v>399.83300000000003</v>
+      </c>
+      <c r="AB39">
+        <v>434.75299999999999</v>
+      </c>
+      <c r="AC39">
+        <v>470.83800000000002</v>
+      </c>
+      <c r="AD39">
+        <v>511.548</v>
+      </c>
+      <c r="AE39">
+        <v>551.00300000000004</v>
+      </c>
+      <c r="AF39">
+        <v>592.02800000000002</v>
+      </c>
+      <c r="AG39">
+        <v>634.52300000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40">
+        <v>25.57</v>
+      </c>
+      <c r="C40">
+        <v>33.991999999999997</v>
+      </c>
+      <c r="D40">
+        <v>42.414000000000001</v>
+      </c>
+      <c r="E40">
+        <v>51.006</v>
+      </c>
+      <c r="F40">
+        <v>58.975999999999999</v>
+      </c>
+      <c r="G40">
+        <v>70.212000000000003</v>
+      </c>
+      <c r="H40">
+        <v>93.218000000000004</v>
+      </c>
+      <c r="I40">
+        <v>118.994</v>
+      </c>
+      <c r="J40">
+        <v>145.03</v>
+      </c>
+      <c r="K40">
+        <v>183.48400000000001</v>
+      </c>
+      <c r="L40">
+        <v>213.334</v>
+      </c>
+      <c r="M40">
+        <v>238.376</v>
+      </c>
+      <c r="N40">
+        <v>262.99</v>
+      </c>
+      <c r="O40">
+        <v>286.274</v>
+      </c>
+      <c r="P40">
+        <v>317.04399999999998</v>
+      </c>
+      <c r="Q40">
+        <v>354.18799999999999</v>
+      </c>
+      <c r="R40">
+        <v>391.346</v>
+      </c>
+      <c r="S40">
+        <v>426.96</v>
+      </c>
+      <c r="T40">
+        <v>462.34</v>
+      </c>
+      <c r="U40">
+        <v>499.6</v>
+      </c>
+      <c r="V40">
+        <v>533.35799999999995</v>
+      </c>
+      <c r="W40">
+        <v>565.70600000000002</v>
+      </c>
+      <c r="X40">
+        <v>595.98599999999999</v>
+      </c>
+      <c r="Y40">
+        <v>624.202</v>
+      </c>
+      <c r="Z40">
+        <v>645.41800000000001</v>
+      </c>
+      <c r="AA40">
+        <v>664.63199999999995</v>
+      </c>
+      <c r="AB40">
+        <v>680.85400000000004</v>
+      </c>
+      <c r="AC40">
+        <v>693.45</v>
+      </c>
+      <c r="AD40">
+        <v>707.072</v>
+      </c>
+      <c r="AE40">
+        <v>715.11599999999999</v>
+      </c>
+      <c r="AF40">
+        <v>721.35199999999998</v>
+      </c>
+      <c r="AG40">
+        <v>726.08199999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42">
+        <v>2019</v>
+      </c>
+      <c r="C42">
+        <v>2020</v>
+      </c>
+      <c r="D42">
+        <v>2021</v>
+      </c>
+      <c r="E42">
+        <v>2022</v>
+      </c>
+      <c r="F42">
+        <v>2023</v>
+      </c>
+      <c r="G42">
+        <v>2024</v>
+      </c>
+      <c r="H42">
+        <v>2025</v>
+      </c>
+      <c r="I42">
+        <v>2026</v>
+      </c>
+      <c r="J42">
+        <v>2027</v>
+      </c>
+      <c r="K42">
+        <v>2028</v>
+      </c>
+      <c r="L42">
+        <v>2029</v>
+      </c>
+      <c r="M42">
+        <v>2030</v>
+      </c>
+      <c r="N42">
+        <v>2031</v>
+      </c>
+      <c r="O42">
+        <v>2032</v>
+      </c>
+      <c r="P42">
+        <v>2033</v>
+      </c>
+      <c r="Q42">
+        <v>2034</v>
+      </c>
+      <c r="R42">
+        <v>2035</v>
+      </c>
+      <c r="S42">
+        <v>2036</v>
+      </c>
+      <c r="T42">
+        <v>2037</v>
+      </c>
+      <c r="U42">
+        <v>2038</v>
+      </c>
+      <c r="V42">
+        <v>2039</v>
+      </c>
+      <c r="W42">
+        <v>2040</v>
+      </c>
+      <c r="X42">
+        <v>2041</v>
+      </c>
+      <c r="Y42">
+        <v>2042</v>
+      </c>
+      <c r="Z42">
+        <v>2043</v>
+      </c>
+      <c r="AA42">
+        <v>2044</v>
+      </c>
+      <c r="AB42">
+        <v>2045</v>
+      </c>
+      <c r="AC42">
+        <v>2046</v>
+      </c>
+      <c r="AD42">
+        <v>2047</v>
+      </c>
+      <c r="AE42">
+        <v>2048</v>
+      </c>
+      <c r="AF42">
+        <v>2049</v>
+      </c>
+      <c r="AG42">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43">
+        <v>1.5697200000000001E-2</v>
+      </c>
+      <c r="C43">
+        <v>1.3069900000000001E-2</v>
+      </c>
+      <c r="D43">
+        <v>1.21618E-2</v>
+      </c>
+      <c r="E43">
+        <v>1.14193E-2</v>
+      </c>
+      <c r="F43">
+        <v>1.03477E-2</v>
+      </c>
+      <c r="G43">
+        <v>1.0981100000000001E-2</v>
+      </c>
+      <c r="H43">
+        <v>1.1796299999999999E-2</v>
+      </c>
+      <c r="I43">
+        <v>1.2611600000000001E-2</v>
+      </c>
+      <c r="J43">
+        <v>1.3473199999999999E-2</v>
+      </c>
+      <c r="K43">
+        <v>9.6616700000000007E-3</v>
+      </c>
+      <c r="L43">
+        <v>6.8585E-3</v>
+      </c>
+      <c r="M43">
+        <v>4.2024999999999996E-3</v>
+      </c>
+      <c r="N43">
+        <v>3.4534499999999998E-3</v>
+      </c>
+      <c r="O43">
+        <v>3.0854799999999998E-3</v>
+      </c>
+      <c r="P43">
+        <v>2.9200699999999999E-3</v>
+      </c>
+      <c r="Q43">
+        <v>2.83899E-3</v>
+      </c>
+      <c r="R43">
+        <v>2.8715899999999998E-3</v>
+      </c>
+      <c r="S43">
+        <v>2.9808500000000002E-3</v>
+      </c>
+      <c r="T43">
+        <v>3.1255100000000002E-3</v>
+      </c>
+      <c r="U43">
+        <v>3.3071200000000002E-3</v>
+      </c>
+      <c r="V43">
+        <v>3.5533800000000001E-3</v>
+      </c>
+      <c r="W43">
+        <v>3.8235500000000002E-3</v>
+      </c>
+      <c r="X43">
+        <v>4.1262399999999998E-3</v>
+      </c>
+      <c r="Y43">
+        <v>4.4641699999999999E-3</v>
+      </c>
+      <c r="Z43">
+        <v>4.77452E-3</v>
+      </c>
+      <c r="AA43">
+        <v>5.1896499999999996E-3</v>
+      </c>
+      <c r="AB43">
+        <v>5.6001499999999999E-3</v>
+      </c>
+      <c r="AC43">
+        <v>6.0639200000000004E-3</v>
+      </c>
+      <c r="AD43">
+        <v>6.5647700000000002E-3</v>
+      </c>
+      <c r="AE43">
+        <v>7.1044400000000001E-3</v>
+      </c>
+      <c r="AF43">
+        <v>7.6543899999999996E-3</v>
+      </c>
+      <c r="AG43">
+        <v>8.1908499999999995E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44">
+        <v>5.8579599999999997E-3</v>
+      </c>
+      <c r="C44">
+        <v>8.5454399999999996E-3</v>
+      </c>
+      <c r="D44">
+        <v>1.1308E-2</v>
+      </c>
+      <c r="E44">
+        <v>1.36633E-2</v>
+      </c>
+      <c r="F44">
+        <v>1.4352999999999999E-2</v>
+      </c>
+      <c r="G44">
+        <v>1.6143999999999999E-2</v>
+      </c>
+      <c r="H44">
+        <v>1.9394399999999999E-2</v>
+      </c>
+      <c r="I44">
+        <v>2.6650900000000002E-2</v>
+      </c>
+      <c r="J44">
+        <v>3.5288100000000003E-2</v>
+      </c>
+      <c r="K44">
+        <v>2.9432699999999999E-2</v>
+      </c>
+      <c r="L44">
+        <v>2.66074E-2</v>
+      </c>
+      <c r="M44">
+        <v>1.9512600000000001E-2</v>
+      </c>
+      <c r="N44">
+        <v>1.7609199999999998E-2</v>
+      </c>
+      <c r="O44">
+        <v>1.6190599999999999E-2</v>
+      </c>
+      <c r="P44">
+        <v>1.50496E-2</v>
+      </c>
+      <c r="Q44">
+        <v>1.44993E-2</v>
+      </c>
+      <c r="R44">
+        <v>1.44739E-2</v>
+      </c>
+      <c r="S44">
+        <v>1.45656E-2</v>
+      </c>
+      <c r="T44">
+        <v>1.4593399999999999E-2</v>
+      </c>
+      <c r="U44">
+        <v>1.46131E-2</v>
+      </c>
+      <c r="V44">
+        <v>1.48086E-2</v>
+      </c>
+      <c r="W44">
+        <v>1.48679E-2</v>
+      </c>
+      <c r="X44">
+        <v>1.48734E-2</v>
+      </c>
+      <c r="Y44">
+        <v>1.48269E-2</v>
+      </c>
+      <c r="Z44">
+        <v>1.4567099999999999E-2</v>
+      </c>
+      <c r="AA44">
+        <v>1.44066E-2</v>
+      </c>
+      <c r="AB44">
+        <v>1.41154E-2</v>
+      </c>
+      <c r="AC44">
+        <v>1.3835999999999999E-2</v>
+      </c>
+      <c r="AD44">
+        <v>1.35409E-2</v>
+      </c>
+      <c r="AE44">
+        <v>1.32149E-2</v>
+      </c>
+      <c r="AF44">
+        <v>1.28722E-2</v>
+      </c>
+      <c r="AG44">
+        <v>1.24653E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A46" s="13">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47">
+        <v>2019</v>
+      </c>
+      <c r="C47">
+        <v>2020</v>
+      </c>
+      <c r="D47">
+        <v>2021</v>
+      </c>
+      <c r="E47">
+        <v>2022</v>
+      </c>
+      <c r="F47">
+        <v>2023</v>
+      </c>
+      <c r="G47">
+        <v>2024</v>
+      </c>
+      <c r="H47">
+        <v>2025</v>
+      </c>
+      <c r="I47">
+        <v>2026</v>
+      </c>
+      <c r="J47">
+        <v>2027</v>
+      </c>
+      <c r="K47">
+        <v>2028</v>
+      </c>
+      <c r="L47">
+        <v>2029</v>
+      </c>
+      <c r="M47">
+        <v>2030</v>
+      </c>
+      <c r="N47">
+        <v>2031</v>
+      </c>
+      <c r="O47">
+        <v>2032</v>
+      </c>
+      <c r="P47">
+        <v>2033</v>
+      </c>
+      <c r="Q47">
+        <v>2034</v>
+      </c>
+      <c r="R47">
+        <v>2035</v>
+      </c>
+      <c r="S47">
+        <v>2036</v>
+      </c>
+      <c r="T47">
+        <v>2037</v>
+      </c>
+      <c r="U47">
+        <v>2038</v>
+      </c>
+      <c r="V47">
+        <v>2039</v>
+      </c>
+      <c r="W47">
+        <v>2040</v>
+      </c>
+      <c r="X47">
+        <v>2041</v>
+      </c>
+      <c r="Y47">
+        <v>2042</v>
+      </c>
+      <c r="Z47">
+        <v>2043</v>
+      </c>
+      <c r="AA47">
+        <v>2044</v>
+      </c>
+      <c r="AB47">
+        <v>2045</v>
+      </c>
+      <c r="AC47">
+        <v>2046</v>
+      </c>
+      <c r="AD47">
+        <v>2047</v>
+      </c>
+      <c r="AE47">
+        <v>2048</v>
+      </c>
+      <c r="AF47">
+        <v>2049</v>
+      </c>
+      <c r="AG47">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>35.213000000000001</v>
+      </c>
+      <c r="C48">
+        <v>37.707999999999998</v>
+      </c>
+      <c r="D48">
+        <v>40.203000000000003</v>
+      </c>
+      <c r="E48">
+        <v>43.718000000000004</v>
+      </c>
+      <c r="F48">
+        <v>48.783000000000001</v>
+      </c>
+      <c r="G48">
+        <v>54.667999999999999</v>
+      </c>
+      <c r="H48">
+        <v>60.497999999999998</v>
+      </c>
+      <c r="I48">
+        <v>66.313000000000002</v>
+      </c>
+      <c r="J48">
+        <v>72.828000000000003</v>
+      </c>
+      <c r="K48">
+        <v>78.763000000000005</v>
+      </c>
+      <c r="L48">
+        <v>83.048000000000002</v>
+      </c>
+      <c r="M48">
+        <v>87.278000000000006</v>
+      </c>
+      <c r="N48">
+        <v>93.412999999999997</v>
+      </c>
+      <c r="O48">
+        <v>102.108</v>
+      </c>
+      <c r="P48">
+        <v>115.018</v>
+      </c>
+      <c r="Q48">
+        <v>129.928</v>
+      </c>
+      <c r="R48">
+        <v>146.06800000000001</v>
+      </c>
+      <c r="S48">
+        <v>163.35300000000001</v>
+      </c>
+      <c r="T48">
+        <v>182.19800000000001</v>
+      </c>
+      <c r="U48">
+        <v>203.238</v>
+      </c>
+      <c r="V48">
+        <v>225.59299999999999</v>
+      </c>
+      <c r="W48">
+        <v>249.88300000000001</v>
+      </c>
+      <c r="X48">
+        <v>276.13799999999998</v>
+      </c>
+      <c r="Y48">
+        <v>304.52800000000002</v>
+      </c>
+      <c r="Z48">
+        <v>333.41800000000001</v>
+      </c>
+      <c r="AA48">
+        <v>364.65800000000002</v>
+      </c>
+      <c r="AB48">
+        <v>397.77800000000002</v>
+      </c>
+      <c r="AC48">
+        <v>432.24299999999999</v>
+      </c>
+      <c r="AD48">
+        <v>471.22300000000001</v>
+      </c>
+      <c r="AE48">
+        <v>509.34800000000001</v>
+      </c>
+      <c r="AF48">
+        <v>549.26800000000003</v>
+      </c>
+      <c r="AG48">
+        <v>590.85299999999995</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <v>25.57</v>
+      </c>
+      <c r="C49">
+        <v>33.991999999999997</v>
+      </c>
+      <c r="D49">
+        <v>42.414000000000001</v>
+      </c>
+      <c r="E49">
+        <v>50.9</v>
+      </c>
+      <c r="F49">
+        <v>58.997999999999998</v>
+      </c>
+      <c r="G49">
+        <v>70.638000000000005</v>
+      </c>
+      <c r="H49">
+        <v>94.668000000000006</v>
+      </c>
+      <c r="I49">
+        <v>123.474</v>
+      </c>
+      <c r="J49">
+        <v>157.08000000000001</v>
+      </c>
+      <c r="K49">
+        <v>198.066</v>
+      </c>
+      <c r="L49">
+        <v>230.00399999999999</v>
+      </c>
+      <c r="M49">
+        <v>258.86799999999999</v>
+      </c>
+      <c r="N49">
+        <v>288.98399999999998</v>
+      </c>
+      <c r="O49">
+        <v>316.29199999999997</v>
+      </c>
+      <c r="P49">
+        <v>348.702</v>
+      </c>
+      <c r="Q49">
+        <v>387.45</v>
+      </c>
+      <c r="R49">
+        <v>426.27199999999999</v>
+      </c>
+      <c r="S49">
+        <v>463.61799999999999</v>
+      </c>
+      <c r="T49">
+        <v>500.83600000000001</v>
+      </c>
+      <c r="U49">
+        <v>540.11400000000003</v>
+      </c>
+      <c r="V49">
+        <v>575.904</v>
+      </c>
+      <c r="W49">
+        <v>610.36800000000005</v>
+      </c>
+      <c r="X49">
+        <v>642.87400000000002</v>
+      </c>
+      <c r="Y49">
+        <v>673.36400000000003</v>
+      </c>
+      <c r="Z49">
+        <v>696.75</v>
+      </c>
+      <c r="AA49">
+        <v>718.26400000000001</v>
+      </c>
+      <c r="AB49">
+        <v>736.68799999999999</v>
+      </c>
+      <c r="AC49">
+        <v>751.33600000000001</v>
+      </c>
+      <c r="AD49">
+        <v>767.10799999999995</v>
+      </c>
+      <c r="AE49">
+        <v>776.80799999999999</v>
+      </c>
+      <c r="AF49">
+        <v>784.49400000000003</v>
+      </c>
+      <c r="AG49">
+        <v>790.428</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51">
+        <v>2019</v>
+      </c>
+      <c r="C51">
+        <v>2020</v>
+      </c>
+      <c r="D51">
+        <v>2021</v>
+      </c>
+      <c r="E51">
+        <v>2022</v>
+      </c>
+      <c r="F51">
+        <v>2023</v>
+      </c>
+      <c r="G51">
+        <v>2024</v>
+      </c>
+      <c r="H51">
+        <v>2025</v>
+      </c>
+      <c r="I51">
+        <v>2026</v>
+      </c>
+      <c r="J51">
+        <v>2027</v>
+      </c>
+      <c r="K51">
+        <v>2028</v>
+      </c>
+      <c r="L51">
+        <v>2029</v>
+      </c>
+      <c r="M51">
+        <v>2030</v>
+      </c>
+      <c r="N51">
+        <v>2031</v>
+      </c>
+      <c r="O51">
+        <v>2032</v>
+      </c>
+      <c r="P51">
+        <v>2033</v>
+      </c>
+      <c r="Q51">
+        <v>2034</v>
+      </c>
+      <c r="R51">
+        <v>2035</v>
+      </c>
+      <c r="S51">
+        <v>2036</v>
+      </c>
+      <c r="T51">
+        <v>2037</v>
+      </c>
+      <c r="U51">
+        <v>2038</v>
+      </c>
+      <c r="V51">
+        <v>2039</v>
+      </c>
+      <c r="W51">
+        <v>2040</v>
+      </c>
+      <c r="X51">
+        <v>2041</v>
+      </c>
+      <c r="Y51">
+        <v>2042</v>
+      </c>
+      <c r="Z51">
+        <v>2043</v>
+      </c>
+      <c r="AA51">
+        <v>2044</v>
+      </c>
+      <c r="AB51">
+        <v>2045</v>
+      </c>
+      <c r="AC51">
+        <v>2046</v>
+      </c>
+      <c r="AD51">
+        <v>2047</v>
+      </c>
+      <c r="AE51">
+        <v>2048</v>
+      </c>
+      <c r="AF51">
+        <v>2049</v>
+      </c>
+      <c r="AG51">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52">
+        <v>1.5697200000000001E-2</v>
+      </c>
+      <c r="C52">
+        <v>1.3069900000000001E-2</v>
+      </c>
+      <c r="D52">
+        <v>1.13703E-2</v>
+      </c>
+      <c r="E52">
+        <v>9.9699100000000002E-3</v>
+      </c>
+      <c r="F52">
+        <v>8.3124700000000006E-3</v>
+      </c>
+      <c r="G52">
+        <v>8.2406800000000002E-3</v>
+      </c>
+      <c r="H52">
+        <v>8.4487599999999996E-3</v>
+      </c>
+      <c r="I52">
+        <v>8.8629999999999994E-3</v>
+      </c>
+      <c r="J52">
+        <v>9.34047E-3</v>
+      </c>
+      <c r="K52">
+        <v>6.5173999999999996E-3</v>
+      </c>
+      <c r="L52">
+        <v>4.0959400000000002E-3</v>
+      </c>
+      <c r="M52">
+        <v>2.2174899999999999E-3</v>
+      </c>
+      <c r="N52">
+        <v>1.5962999999999999E-3</v>
+      </c>
+      <c r="O52">
+        <v>1.21301E-3</v>
+      </c>
+      <c r="P52">
+        <v>1.0335399999999999E-3</v>
+      </c>
+      <c r="Q52">
+        <v>1.01431E-3</v>
+      </c>
+      <c r="R52">
+        <v>1.06083E-3</v>
+      </c>
+      <c r="S52">
+        <v>1.1533100000000001E-3</v>
+      </c>
+      <c r="T52">
+        <v>1.26516E-3</v>
+      </c>
+      <c r="U52">
+        <v>1.40077E-3</v>
+      </c>
+      <c r="V52">
+        <v>1.5767000000000001E-3</v>
+      </c>
+      <c r="W52">
+        <v>1.7675099999999999E-3</v>
+      </c>
+      <c r="X52">
+        <v>1.9795799999999999E-3</v>
+      </c>
+      <c r="Y52">
+        <v>2.2138399999999999E-3</v>
+      </c>
+      <c r="Z52">
+        <v>2.4328599999999998E-3</v>
+      </c>
+      <c r="AA52">
+        <v>2.7223500000000001E-3</v>
+      </c>
+      <c r="AB52">
+        <v>3.01133E-3</v>
+      </c>
+      <c r="AC52">
+        <v>3.3380800000000002E-3</v>
+      </c>
+      <c r="AD52">
+        <v>3.6909500000000001E-3</v>
+      </c>
+      <c r="AE52">
+        <v>4.0730000000000002E-3</v>
+      </c>
+      <c r="AF52">
+        <v>4.46576E-3</v>
+      </c>
+      <c r="AG52">
+        <v>4.8538599999999998E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53">
+        <v>5.8579599999999997E-3</v>
+      </c>
+      <c r="C53">
+        <v>8.5454399999999996E-3</v>
+      </c>
+      <c r="D53">
+        <v>1.0567999999999999E-2</v>
+      </c>
+      <c r="E53">
+        <v>7.8869100000000004E-3</v>
+      </c>
+      <c r="F53">
+        <v>1.17255E-2</v>
+      </c>
+      <c r="G53">
+        <v>1.23888E-2</v>
+      </c>
+      <c r="H53">
+        <v>1.40564E-2</v>
+      </c>
+      <c r="I53">
+        <v>1.96326E-2</v>
+      </c>
+      <c r="J53">
+        <v>2.6854900000000001E-2</v>
+      </c>
+      <c r="K53">
+        <v>2.3935100000000001E-2</v>
+      </c>
+      <c r="L53">
+        <v>2.0309299999999999E-2</v>
+      </c>
+      <c r="M53">
+        <v>1.5114000000000001E-2</v>
+      </c>
+      <c r="N53">
+        <v>1.38785E-2</v>
+      </c>
+      <c r="O53">
+        <v>1.2937499999999999E-2</v>
+      </c>
+      <c r="P53">
+        <v>1.2093700000000001E-2</v>
+      </c>
+      <c r="Q53">
+        <v>1.16039E-2</v>
+      </c>
+      <c r="R53">
+        <v>1.1510599999999999E-2</v>
+      </c>
+      <c r="S53">
+        <v>1.15275E-2</v>
+      </c>
+      <c r="T53">
+        <v>1.15035E-2</v>
+      </c>
+      <c r="U53">
+        <v>1.1487300000000001E-2</v>
+      </c>
+      <c r="V53">
+        <v>1.16077E-2</v>
+      </c>
+      <c r="W53">
+        <v>1.1632699999999999E-2</v>
+      </c>
+      <c r="X53">
+        <v>1.1623100000000001E-2</v>
+      </c>
+      <c r="Y53">
+        <v>1.1576299999999999E-2</v>
+      </c>
+      <c r="Z53">
+        <v>1.13732E-2</v>
+      </c>
+      <c r="AA53">
+        <v>1.1262899999999999E-2</v>
+      </c>
+      <c r="AB53">
+        <v>1.1052899999999999E-2</v>
+      </c>
+      <c r="AC53">
+        <v>1.0855699999999999E-2</v>
+      </c>
+      <c r="AD53">
+        <v>1.06439E-2</v>
+      </c>
+      <c r="AE53">
+        <v>1.0408199999999999E-2</v>
+      </c>
+      <c r="AF53">
+        <v>1.0157599999999999E-2</v>
+      </c>
+      <c r="AG53">
+        <v>9.8524000000000007E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1169,8 +2369,8 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <f>Calibration!B22</f>
-        <v>0.5</v>
+        <f>Calibration!B20</f>
+        <v>0.42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>